<commit_message>
eerste versie enquete conversie werkt
</commit_message>
<xml_diff>
--- a/studenten.xlsx
+++ b/studenten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aapa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164CADA4-8F23-4309-8CA4-FA61DDB6B5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5CF2BB-3EA6-4585-AB46-601FD773A44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E5AA04ED-8130-4B05-9B27-AA2E1C80DA6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{E5AA04ED-8130-4B05-9B27-AA2E1C80DA6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -1526,7 +1526,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1848,8 +1848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4A00D2-AAB1-47C6-A33A-830D16EB55BE}">
   <dimension ref="A1:E167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82:XFD82"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1857,8 +1857,8 @@
     <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>